<commit_message>
Coords class == Position class. Position unit tests - 1 failing
</commit_message>
<xml_diff>
--- a/Coords_Patterns.xlsx
+++ b/Coords_Patterns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Linda.Johnstone/Documents/fma/TicTacToe2D/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08604B31-5CB4-124C-9420-4A4F4746458A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{485F7260-962F-3B4B-A931-942FD27E2D8C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{2544AC0C-3621-D94F-BC29-F5F8A44176B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
   <si>
     <t>Plus</t>
   </si>
@@ -42,60 +42,15 @@
     <t>Multiply</t>
   </si>
   <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>01</t>
-  </si>
-  <si>
     <t>10</t>
   </si>
   <si>
     <t>11</t>
   </si>
   <si>
-    <t>110</t>
-  </si>
-  <si>
-    <t>1000</t>
-  </si>
-  <si>
-    <t>1001</t>
-  </si>
-  <si>
-    <t>1010</t>
-  </si>
-  <si>
     <t>Custom (xy)</t>
   </si>
   <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>010</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
@@ -150,9 +105,6 @@
     <t>29</t>
   </si>
   <si>
-    <t>210</t>
-  </si>
-  <si>
     <t>30</t>
   </si>
   <si>
@@ -183,9 +135,6 @@
     <t>39</t>
   </si>
   <si>
-    <t>310</t>
-  </si>
-  <si>
     <t>40</t>
   </si>
   <si>
@@ -216,9 +165,6 @@
     <t>49</t>
   </si>
   <si>
-    <t>410</t>
-  </si>
-  <si>
     <t>50</t>
   </si>
   <si>
@@ -249,9 +195,6 @@
     <t>59</t>
   </si>
   <si>
-    <t>510</t>
-  </si>
-  <si>
     <t>60</t>
   </si>
   <si>
@@ -282,9 +225,6 @@
     <t>69</t>
   </si>
   <si>
-    <t>610</t>
-  </si>
-  <si>
     <t>70</t>
   </si>
   <si>
@@ -315,9 +255,6 @@
     <t>79</t>
   </si>
   <si>
-    <t>710</t>
-  </si>
-  <si>
     <t>80</t>
   </si>
   <si>
@@ -351,9 +288,6 @@
     <t>90</t>
   </si>
   <si>
-    <t>810</t>
-  </si>
-  <si>
     <t>91</t>
   </si>
   <si>
@@ -381,33 +315,6 @@
     <t>99</t>
   </si>
   <si>
-    <t>910</t>
-  </si>
-  <si>
-    <t>1002</t>
-  </si>
-  <si>
-    <t>1003</t>
-  </si>
-  <si>
-    <t>1004</t>
-  </si>
-  <si>
-    <t>1005</t>
-  </si>
-  <si>
-    <t>1006</t>
-  </si>
-  <si>
-    <t>1007</t>
-  </si>
-  <si>
-    <t>1008</t>
-  </si>
-  <si>
-    <t>1009</t>
-  </si>
-  <si>
     <t>Pattern</t>
   </si>
   <si>
@@ -417,10 +324,10 @@
     <t>x * y</t>
   </si>
   <si>
-    <t>except for x = 10 &amp; y = 10</t>
-  </si>
-  <si>
     <t>x * 10 + y</t>
+  </si>
+  <si>
+    <t>107</t>
   </si>
 </sst>
 </file>
@@ -478,7 +385,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -489,13 +396,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -815,14 +731,14 @@
   <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="12" width="10.83203125" style="2"/>
-    <col min="13" max="13" width="21.5" style="6" customWidth="1"/>
+    <col min="13" max="13" width="21.5" style="5" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
@@ -873,8 +789,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
-        <v>124</v>
+      <c r="M1" s="4" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -915,8 +831,8 @@
       <c r="L2" s="2">
         <v>10</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>125</v>
+      <c r="M2" s="5" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -1504,8 +1420,8 @@
       <c r="L15" s="2">
         <v>0</v>
       </c>
-      <c r="M15" s="6" t="s">
-        <v>126</v>
+      <c r="M15" s="5" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -1918,491 +1834,497 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B27" s="3">
-        <v>0</v>
-      </c>
-      <c r="C27" s="3">
+        <v>4</v>
+      </c>
+      <c r="B27" s="6">
+        <v>0</v>
+      </c>
+      <c r="C27" s="6">
         <f>B27+1</f>
         <v>1</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="6">
         <f t="shared" ref="D27:L27" si="12">C27+1</f>
         <v>2</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="6">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="F27" s="3">
+      <c r="F27" s="6">
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="G27" s="3">
+      <c r="G27" s="6">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="H27" s="3">
+      <c r="H27" s="6">
         <f t="shared" si="12"/>
         <v>6</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="6">
         <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="6">
         <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="6">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="L27" s="3">
+      <c r="L27" s="6">
         <f t="shared" si="12"/>
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
-        <v>0</v>
-      </c>
-      <c r="B28" s="4" t="s">
+    <row r="28" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>0</v>
+      </c>
+      <c r="B28" s="7">
+        <v>0</v>
+      </c>
+      <c r="C28" s="7">
+        <v>1</v>
+      </c>
+      <c r="D28" s="7">
         <v>2</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="E28" s="7">
         <v>3</v>
       </c>
-      <c r="D28" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G28" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L28" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="M28" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="F28" s="7">
+        <v>4</v>
+      </c>
+      <c r="G28" s="7">
+        <v>5</v>
+      </c>
+      <c r="H28" s="7">
+        <v>6</v>
+      </c>
+      <c r="I28" s="7">
+        <v>7</v>
+      </c>
+      <c r="J28" s="7">
+        <v>8</v>
+      </c>
+      <c r="K28" s="7">
+        <v>9</v>
+      </c>
+      <c r="L28" s="7">
+        <v>10</v>
+      </c>
+      <c r="M28" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
         <f>A28+1</f>
         <v>1</v>
       </c>
-      <c r="B29" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="B29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="8">
         <v>20</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I29" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="L29" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    </row>
+    <row r="30" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
         <f t="shared" ref="A30:A37" si="13">A29+1</f>
         <v>2</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="4" t="s">
+      <c r="B30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J30" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="L30" s="8">
         <v>30</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K30" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="L30" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="M30" s="9"/>
+    </row>
+    <row r="31" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
         <f t="shared" si="13"/>
         <v>3</v>
       </c>
-      <c r="B31" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C31" s="4" t="s">
+      <c r="B31" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J31" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="L31" s="8">
         <v>40</v>
       </c>
-      <c r="D31" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I31" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L31" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="M31" s="9"/>
+    </row>
+    <row r="32" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="6">
         <f t="shared" si="13"/>
         <v>4</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I32" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="J32" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="L32" s="8">
         <v>50</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F32" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="K32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A33" s="3">
+      <c r="M32" s="9"/>
+    </row>
+    <row r="33" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="6">
         <f t="shared" si="13"/>
         <v>5</v>
       </c>
-      <c r="B33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C33" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F33" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="H33" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K33" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="L33" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="B33" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I33" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="K33" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="L33" s="8">
+        <v>60</v>
+      </c>
+      <c r="M33" s="9"/>
+    </row>
+    <row r="34" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="6">
         <f t="shared" si="13"/>
         <v>6</v>
       </c>
-      <c r="B34" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D34" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="L34" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="B34" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="K34" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="L34" s="8">
+        <v>70</v>
+      </c>
+      <c r="M34" s="9"/>
+    </row>
+    <row r="35" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="6">
         <f t="shared" si="13"/>
         <v>7</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="G35" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="K35" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="L35" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="B35" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="D35" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J35" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K35" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L35" s="8">
+        <v>80</v>
+      </c>
+      <c r="M35" s="9"/>
+    </row>
+    <row r="36" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="6">
         <f t="shared" si="13"/>
         <v>8</v>
       </c>
-      <c r="B36" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="L36" s="4" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="B36" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D36" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F36" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="J36" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="L36" s="8">
+        <v>90</v>
+      </c>
+      <c r="M36" s="9"/>
+    </row>
+    <row r="37" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="6">
         <f t="shared" si="13"/>
         <v>9</v>
       </c>
-      <c r="B37" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="E37" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="L37" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="B37" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J37" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="K37" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="L37" s="8">
+        <v>100</v>
+      </c>
+      <c r="M37" s="9"/>
+    </row>
+    <row r="38" spans="1:13" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="6">
         <f>A37+1</f>
         <v>10</v>
       </c>
-      <c r="B38" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G38" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="L38" s="4" t="s">
-        <v>9</v>
-      </c>
+      <c r="B38" s="8">
+        <v>100</v>
+      </c>
+      <c r="C38" s="8">
+        <v>101</v>
+      </c>
+      <c r="D38" s="8">
+        <v>102</v>
+      </c>
+      <c r="E38" s="8">
+        <v>103</v>
+      </c>
+      <c r="F38" s="8">
+        <v>104</v>
+      </c>
+      <c r="G38" s="8">
+        <v>105</v>
+      </c>
+      <c r="H38" s="8">
+        <v>106</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="J38" s="8">
+        <v>108</v>
+      </c>
+      <c r="K38" s="8">
+        <v>109</v>
+      </c>
+      <c r="L38" s="8">
+        <v>110</v>
+      </c>
+      <c r="M38" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B28:L38" numberStoredAsText="1"/>
+    <ignoredError sqref="B29:K29 B30:K30 B31:K31 B32:K32 B33:K33 B34:K34 B35:K35 B36:K36 B37:K37 I38" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>